<commit_message>
converted selesynia cube to a khans tri color cube
</commit_message>
<xml_diff>
--- a/cube_building.xlsx
+++ b/cube_building.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="283">
   <si>
     <t>Card name</t>
   </si>
@@ -860,6 +860,15 @@
   </si>
   <si>
     <t>CMD</t>
+  </si>
+  <si>
+    <t>Narset, Enlightened Master</t>
+  </si>
+  <si>
+    <t>Sidisi, Blood Tyrant</t>
+  </si>
+  <si>
+    <t>Ascendancy</t>
   </si>
 </sst>
 </file>
@@ -868,7 +877,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -1188,7 +1197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1349,6 +1358,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1394,21 +1412,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1426,6 +1444,8 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5800,7 +5820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
@@ -6030,7 +6050,7 @@
         <v>265</v>
       </c>
       <c r="G17" s="19">
-        <f t="shared" ref="G17:G20" si="0">I$16</f>
+        <f t="shared" ref="G17:G19" si="0">I$16</f>
         <v>56</v>
       </c>
       <c r="H17" s="19" t="s">
@@ -6136,132 +6156,151 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="19" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="2" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2" style="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="21"/>
+      <c r="C1" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="J1" s="22"/>
+      <c r="K1" s="2" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="I2" t="s">
+        <v>281</v>
+      </c>
+      <c r="K2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="B3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="F3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>179</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>215</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="G4" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>187</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>211</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="G5" s="19" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>227</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>200</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="G7" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="E7" t="s">
+      <c r="I7" t="s">
         <v>233</v>
       </c>
-      <c r="F7" t="s">
+      <c r="K7" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="19" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G8" s="19" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="19" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G9" s="19" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10" s="19" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G10" s="19" t="s">
         <v>275</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B1:B6">
-    <sortCondition ref="B1"/>
+  <sortState ref="C1:C6">
+    <sortCondition ref="C1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added a new inventory system
</commit_message>
<xml_diff>
--- a/cube_building.xlsx
+++ b/cube_building.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="8265" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="selesynia" sheetId="4" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="Cycles" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">mono!$A$1:$E$27</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">selesynia!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="277">
   <si>
     <t>Card name</t>
   </si>
@@ -544,9 +545,6 @@
     <t>Aura Shards</t>
   </si>
   <si>
-    <t>Brace for Impact</t>
-  </si>
-  <si>
     <t>Brilliant Spectrum</t>
   </si>
   <si>
@@ -568,12 +566,6 @@
     <t>Elderwood Scion</t>
   </si>
   <si>
-    <t>Enigma Eidolon</t>
-  </si>
-  <si>
-    <t>Entropic Eidolon</t>
-  </si>
-  <si>
     <t>Exert Influence</t>
   </si>
   <si>
@@ -652,15 +644,9 @@
     <t>Renounce the Guilds</t>
   </si>
   <si>
-    <t>Roilmage's Trick</t>
-  </si>
-  <si>
     <t>Ruhan of the Fomori</t>
   </si>
   <si>
-    <t>Sandstorm Eidolon</t>
-  </si>
-  <si>
     <t>Seal of the Guildpact</t>
   </si>
   <si>
@@ -713,9 +699,6 @@
   </si>
   <si>
     <t>Vec Townships</t>
-  </si>
-  <si>
-    <t>Verdant Eidolon</t>
   </si>
   <si>
     <t>Victual Sliver</t>
@@ -1814,7 +1797,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="11"/>
@@ -1822,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1994,7 +1977,7 @@
         <v>54</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I9" s="4">
         <v>0.19</v>
@@ -2014,7 +1997,7 @@
         <v>55</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I10" s="9">
         <v>0.2</v>
@@ -2358,7 +2341,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D26" s="4">
         <v>0.15</v>
@@ -2700,7 +2683,7 @@
         <v>86</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="I41" s="4">
         <v>0.24</v>
@@ -2723,7 +2706,7 @@
         <v>87</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="I42" s="4">
         <v>0.24</v>
@@ -2754,7 +2737,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D44" s="4">
         <v>0.17</v>
@@ -2848,14 +2831,14 @@
         <v>0</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="F48" s="12"/>
       <c r="H48" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2964,7 +2947,7 @@
         <v>143</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="I53" s="4">
         <v>1.1299999999999999</v>
@@ -2975,7 +2958,7 @@
         <v>98</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D54" s="4">
         <v>0.3</v>
@@ -2997,7 +2980,7 @@
         <v>99</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D55" s="9">
         <v>0.32</v>
@@ -3028,7 +3011,7 @@
         <v>146</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="I56" s="4">
         <v>1.32</v>
@@ -3073,7 +3056,7 @@
         <v>148</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I58" s="4">
         <v>1.47</v>
@@ -3153,7 +3136,7 @@
         <v>106</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D62" s="4">
         <v>0.35</v>
@@ -3222,7 +3205,7 @@
         <v>109</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D65" s="9">
         <v>0.37</v>
@@ -3388,7 +3371,7 @@
         <v>162</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="I72" s="4">
         <v>2.5499999999999998</v>
@@ -3423,7 +3406,7 @@
         <v>118</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D74" s="4">
         <v>0.46</v>
@@ -3433,7 +3416,7 @@
         <v>164</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I74" s="4">
         <v>2.92</v>
@@ -3541,7 +3524,7 @@
         <v>169</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="I79" s="4">
         <v>4.26</v>
@@ -3684,7 +3667,7 @@
         <v>130</v>
       </c>
       <c r="C86" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D86" s="4">
         <v>0.65</v>
@@ -3705,7 +3688,7 @@
         <v>131</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D87" s="4">
         <v>0.68</v>
@@ -3768,7 +3751,7 @@
         <v>134</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D90" s="9">
         <v>0.72</v>
@@ -3858,7 +3841,7 @@
         <v>138</v>
       </c>
       <c r="C94" s="15" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D94" s="4">
         <v>0.87</v>
@@ -3881,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -3890,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E96" s="5"/>
       <c r="F96" s="12"/>
@@ -3901,7 +3884,7 @@
         <v>185</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D97" s="4">
         <v>12.57</v>
@@ -5557,10 +5540,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5577,33 +5560,33 @@
         <v>0</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="D2" s="9"/>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>1</v>
-      </c>
+      <c r="A3" s="6"/>
       <c r="C3" t="s">
-        <v>195</v>
+        <v>177</v>
+      </c>
+      <c r="D3">
+        <v>3.98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
+      <c r="A4" s="6"/>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -5611,37 +5594,49 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6">
+        <v>1</v>
+      </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>180</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
       <c r="C10" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -5649,169 +5644,147 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
       <c r="C13" t="s">
-        <v>203</v>
-      </c>
-      <c r="D13">
-        <v>3.44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>246</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="C14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D14">
+        <v>3.44</v>
+      </c>
+      <c r="E14" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="C17" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="C15" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="C16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="C18" t="s">
-        <v>212</v>
-      </c>
-    </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6">
+        <v>1</v>
+      </c>
       <c r="C19" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="C20" t="s">
-        <v>219</v>
+        <v>208</v>
+      </c>
+      <c r="E20" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="6">
+        <v>1</v>
+      </c>
       <c r="C21" t="s">
-        <v>229</v>
-      </c>
-      <c r="E21" t="s">
-        <v>245</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="C22" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="6">
+        <v>1</v>
+      </c>
       <c r="C23" t="s">
-        <v>213</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>1</v>
-      </c>
+      <c r="A24" s="6"/>
       <c r="C24" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+      <c r="A25" s="6">
+        <v>1</v>
+      </c>
       <c r="C25" t="s">
-        <v>175</v>
+        <v>223</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="C26" t="s">
-        <v>178</v>
-      </c>
-      <c r="D26">
-        <v>3.98</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>246</v>
+        <v>224</v>
+      </c>
+      <c r="E26" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+      <c r="A27" s="6">
+        <v>1</v>
+      </c>
       <c r="C27" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="C28" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="C29" t="s">
-        <v>206</v>
-      </c>
-      <c r="E29" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="C30" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="C31" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="C33" t="s">
-        <v>234</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:E27">
+    <sortState ref="A2:E33">
+      <sortCondition ref="C1:C33"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5829,23 +5802,23 @@
     <row r="1" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="F2">
         <f>32-4</f>
         <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="I2">
         <f>(360-F2)/5</f>
@@ -5854,30 +5827,30 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F3" s="19">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F4" s="19">
         <v>0</v>
@@ -5885,13 +5858,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F5" s="19">
         <v>0</v>
@@ -5899,13 +5872,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F6" s="19">
         <v>0</v>
@@ -5913,13 +5886,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F7" s="19">
         <v>0</v>
@@ -5927,13 +5900,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F8" s="19">
         <v>0</v>
@@ -5941,16 +5914,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F9" s="19">
         <v>0</v>
@@ -5958,16 +5931,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F10" s="19">
         <v>0</v>
@@ -5975,16 +5948,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F11" s="19">
         <v>0</v>
@@ -5992,16 +5965,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F12" s="19">
         <v>0</v>
@@ -6015,31 +5988,31 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="19" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="E15" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="G16">
         <f>I$16</f>
         <v>56</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="I16">
         <v>56</v>
@@ -6047,14 +6020,14 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G17" s="19">
         <f t="shared" ref="G17:G19" si="0">I$16</f>
         <v>56</v>
       </c>
       <c r="H17" s="19" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="I17">
         <v>10</v>
@@ -6062,14 +6035,14 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="G18" s="19">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="H18" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I18">
         <f>G27-SUM(G16:G26)</f>
@@ -6078,7 +6051,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="G19" s="19">
         <f t="shared" si="0"/>
@@ -6087,7 +6060,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="G20" s="19">
         <f>I$16</f>
@@ -6096,7 +6069,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G21">
         <f>I$17</f>
@@ -6105,7 +6078,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="G22" s="19">
         <f t="shared" ref="G22:G25" si="1">I$17</f>
@@ -6114,7 +6087,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="G23" s="19">
         <f t="shared" si="1"/>
@@ -6123,7 +6096,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="G24" s="19">
         <f>I$17+1</f>
@@ -6132,7 +6105,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G25" s="19">
         <f t="shared" si="1"/>
@@ -6158,7 +6131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -6180,48 +6153,48 @@
     <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="21"/>
       <c r="C1" s="2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D1" s="22"/>
       <c r="E1" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="H1" s="22"/>
       <c r="I1" s="2" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="J1" s="22"/>
       <c r="K1" s="2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C2" t="s">
         <v>169</v>
       </c>
       <c r="E2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="I2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="K2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C3" t="s">
         <v>166</v>
@@ -6229,73 +6202,73 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>167</v>
       </c>
       <c r="K4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E5" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="I7" t="s">
         <v>227</v>
       </c>
-      <c r="E7" t="s">
-        <v>200</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="I7" t="s">
-        <v>233</v>
-      </c>
       <c r="K7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G8" s="19" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G9" s="19" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G10" s="19" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>